<commit_message>
Đã add code cho section video popup, đang bị lỗi chưa play video đc, đã fix nút back to top
</commit_message>
<xml_diff>
--- a/Phân chia công việc/template_task.xlsx
+++ b/Phân chia công việc/template_task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Backtotop homepage</t>
+  </si>
+  <si>
+    <t>Section homepage Video popup</t>
   </si>
 </sst>
 </file>
@@ -410,95 +413,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -782,7 +697,7 @@
   <dimension ref="A1:J986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -1049,15 +964,31 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="11"/>
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="12">
+        <v>45540</v>
+      </c>
+      <c r="C11" s="8">
+        <v>45570</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12">
+        <v>45570</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2145,22 +2076,22 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="D2 D4:D14">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H4:H14">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Đã hoàn thiện section video popup
</commit_message>
<xml_diff>
--- a/Phân chia công việc/template_task.xlsx
+++ b/Phân chia công việc/template_task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Section homepage Video popup</t>
+  </si>
+  <si>
+    <t>About page</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -697,7 +711,7 @@
   <dimension ref="A1:J986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -952,15 +966,31 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45601</v>
+      </c>
+      <c r="C10" s="8">
+        <v>45631</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="11"/>
+      <c r="G10" s="12">
+        <v>45631</v>
+      </c>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -982,9 +1012,11 @@
       <c r="F11" s="12">
         <v>45570</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12">
+        <v>45631</v>
+      </c>
       <c r="H11" s="21">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>21</v>
@@ -2076,22 +2108,22 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="D2 D4:D14">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H4:H14">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>